<commit_message>
tested in absence of financing
</commit_message>
<xml_diff>
--- a/run_sheets/oligopoly_heterogeneous_wcap.xlsx
+++ b/run_sheets/oligopoly_heterogeneous_wcap.xlsx
@@ -408,7 +408,7 @@
   <dimension ref="A1:O34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G2:G5"/>
+      <selection activeCell="F5" sqref="F5:F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -498,7 +498,7 @@
         <v>0.99</v>
       </c>
       <c r="G2" s="1">
-        <v>60</v>
+        <v>600</v>
       </c>
       <c r="H2" s="1">
         <v>0.8</v>
@@ -545,7 +545,7 @@
         <v>0.99</v>
       </c>
       <c r="G3" s="1">
-        <v>60</v>
+        <v>600</v>
       </c>
       <c r="H3" s="1">
         <v>0.8</v>
@@ -592,7 +592,7 @@
         <v>0.99</v>
       </c>
       <c r="G4" s="1">
-        <v>60</v>
+        <v>600</v>
       </c>
       <c r="H4" s="1">
         <v>0.8</v>
@@ -636,7 +636,7 @@
         <v>0.5</v>
       </c>
       <c r="F5" s="1">
-        <v>0.99</v>
+        <v>0.2</v>
       </c>
       <c r="G5" s="1">
         <v>60</v>
@@ -683,7 +683,7 @@
         <v>0.5</v>
       </c>
       <c r="F6" s="1">
-        <v>0.99</v>
+        <v>0.2</v>
       </c>
       <c r="G6" s="1">
         <v>60</v>
@@ -730,7 +730,7 @@
         <v>0.5</v>
       </c>
       <c r="F7" s="1">
-        <v>0.99</v>
+        <v>0.2</v>
       </c>
       <c r="G7" s="1">
         <v>60</v>

</xml_diff>

<commit_message>
dynamic calculation of credit capacity and financing visualizaton added.
</commit_message>
<xml_diff>
--- a/run_sheets/oligopoly_heterogeneous_wcap.xlsx
+++ b/run_sheets/oligopoly_heterogeneous_wcap.xlsx
@@ -489,7 +489,7 @@
         <v>1000</v>
       </c>
       <c r="D2" s="2">
-        <v>5.7</v>
+        <v>1.2</v>
       </c>
       <c r="E2" s="2">
         <v>0.5</v>
@@ -504,22 +504,22 @@
         <v>0.8</v>
       </c>
       <c r="I2" s="1">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="J2" s="1">
         <v>2E-3</v>
       </c>
       <c r="K2" s="1">
-        <v>68</v>
+        <v>3</v>
       </c>
       <c r="L2" s="1">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="M2" s="1">
         <v>30</v>
       </c>
       <c r="N2" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="O2" s="1">
         <v>1</v>
@@ -536,7 +536,7 @@
         <v>1500</v>
       </c>
       <c r="D3" s="2">
-        <v>5.7</v>
+        <v>1.2</v>
       </c>
       <c r="E3" s="2">
         <v>0.5</v>
@@ -551,16 +551,16 @@
         <v>0.8</v>
       </c>
       <c r="I3" s="1">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="J3" s="1">
         <v>2E-3</v>
       </c>
       <c r="K3" s="1">
-        <v>68</v>
+        <v>3</v>
       </c>
       <c r="L3" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="M3" s="1">
         <v>30</v>
@@ -583,7 +583,7 @@
         <v>2000</v>
       </c>
       <c r="D4" s="2">
-        <v>5.7</v>
+        <v>1.2</v>
       </c>
       <c r="E4" s="2">
         <v>0.5</v>
@@ -598,22 +598,22 @@
         <v>0.8</v>
       </c>
       <c r="I4" s="1">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="J4" s="1">
         <v>2E-3</v>
       </c>
       <c r="K4" s="1">
-        <v>68</v>
+        <v>3</v>
       </c>
       <c r="L4" s="1">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="M4" s="1">
         <v>30</v>
       </c>
       <c r="N4" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="O4" s="1">
         <v>1</v>
@@ -630,7 +630,7 @@
         <v>3000</v>
       </c>
       <c r="D5" s="3">
-        <v>5.4</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="E5" s="2">
         <v>0.5</v>
@@ -645,16 +645,16 @@
         <v>0.8</v>
       </c>
       <c r="I5" s="1">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="J5" s="1">
         <v>2E-3</v>
       </c>
       <c r="K5" s="1">
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="L5" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="M5" s="1">
         <v>30</v>
@@ -677,7 +677,7 @@
         <v>3500</v>
       </c>
       <c r="D6" s="3">
-        <v>5.4</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="E6" s="2">
         <v>0.5</v>
@@ -692,16 +692,16 @@
         <v>0.8</v>
       </c>
       <c r="I6" s="1">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="J6" s="1">
         <v>2E-3</v>
       </c>
       <c r="K6" s="1">
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="L6" s="1">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="M6" s="1">
         <v>30</v>
@@ -724,7 +724,7 @@
         <v>4000</v>
       </c>
       <c r="D7" s="3">
-        <v>5.4</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="E7" s="2">
         <v>0.5</v>
@@ -739,16 +739,16 @@
         <v>0.8</v>
       </c>
       <c r="I7" s="1">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="J7" s="1">
         <v>2E-3</v>
       </c>
       <c r="K7" s="1">
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="L7" s="1">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="M7" s="1">
         <v>30</v>
@@ -771,7 +771,7 @@
         <v>5000</v>
       </c>
       <c r="D8" s="3">
-        <v>5.0999999999999996</v>
+        <v>1</v>
       </c>
       <c r="E8" s="2">
         <v>0.5</v>
@@ -786,16 +786,16 @@
         <v>0.8</v>
       </c>
       <c r="I8" s="1">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="J8" s="1">
         <v>2E-3</v>
       </c>
       <c r="K8" s="1">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="L8" s="1">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="M8" s="1">
         <v>30</v>
@@ -818,7 +818,7 @@
         <v>5500</v>
       </c>
       <c r="D9" s="3">
-        <v>5.0999999999999996</v>
+        <v>1</v>
       </c>
       <c r="E9" s="2">
         <v>0.5</v>
@@ -833,16 +833,16 @@
         <v>0.8</v>
       </c>
       <c r="I9" s="1">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="J9" s="1">
         <v>2E-3</v>
       </c>
       <c r="K9" s="1">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="L9" s="1">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="M9" s="1">
         <v>30</v>
@@ -865,7 +865,7 @@
         <v>6000</v>
       </c>
       <c r="D10" s="3">
-        <v>5.0999999999999996</v>
+        <v>1</v>
       </c>
       <c r="E10" s="2">
         <v>0.5</v>
@@ -880,16 +880,16 @@
         <v>0.8</v>
       </c>
       <c r="I10" s="1">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="J10" s="1">
         <v>2E-3</v>
       </c>
       <c r="K10" s="1">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="L10" s="1">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="M10" s="1">
         <v>30</v>

</xml_diff>

<commit_message>
initial efforts to add trade credit
</commit_message>
<xml_diff>
--- a/run_sheets/oligopoly_heterogeneous_wcap.xlsx
+++ b/run_sheets/oligopoly_heterogeneous_wcap.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
   <si>
     <t>r</t>
   </si>
@@ -76,6 +76,12 @@
   </si>
   <si>
     <t>fixed_assets</t>
+  </si>
+  <si>
+    <t>payment_term</t>
+  </si>
+  <si>
+    <t>tc_rate</t>
   </si>
 </sst>
 </file>
@@ -408,10 +414,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P34"/>
+  <dimension ref="A1:R34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="R11" sqref="R11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -432,10 +438,11 @@
     <col min="14" max="14" width="13.625" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="13.125" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="11.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="9" style="1"/>
+    <col min="17" max="17" width="12.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -484,8 +491,14 @@
       <c r="P1" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -534,8 +547,14 @@
       <c r="P2" s="1">
         <v>3000</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q2" s="1">
+        <v>10</v>
+      </c>
+      <c r="R2" s="1">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -584,8 +603,14 @@
       <c r="P3" s="1">
         <v>4500</v>
       </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q3" s="1">
+        <v>10</v>
+      </c>
+      <c r="R3" s="1">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -634,8 +659,14 @@
       <c r="P4" s="1">
         <v>6000</v>
       </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q4" s="1">
+        <v>10</v>
+      </c>
+      <c r="R4" s="1">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -684,8 +715,14 @@
       <c r="P5" s="1">
         <v>9000</v>
       </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q5" s="1">
+        <v>10</v>
+      </c>
+      <c r="R5" s="1">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -734,8 +771,14 @@
       <c r="P6" s="1">
         <v>10500</v>
       </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q6" s="1">
+        <v>10</v>
+      </c>
+      <c r="R6" s="1">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -784,8 +827,14 @@
       <c r="P7" s="1">
         <v>12000</v>
       </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q7" s="1">
+        <v>10</v>
+      </c>
+      <c r="R7" s="1">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -834,8 +883,14 @@
       <c r="P8" s="1">
         <v>15000</v>
       </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q8" s="1">
+        <v>10</v>
+      </c>
+      <c r="R8" s="1">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -884,8 +939,14 @@
       <c r="P9" s="1">
         <v>16500</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q9" s="1">
+        <v>10</v>
+      </c>
+      <c r="R9" s="1">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -934,31 +995,37 @@
       <c r="P10" s="1">
         <v>18000</v>
       </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q10" s="1">
+        <v>10</v>
+      </c>
+      <c r="R10" s="1">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="E11" s="2"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B12" s="5"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B13" s="5"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B14" s="5"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B15" s="5"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B16" s="5"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>

</xml_diff>